<commit_message>
Set 1 point for null point value #54
</commit_message>
<xml_diff>
--- a/uploads/excel/modele.xlsx
+++ b/uploads/excel/modele.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="12915" windowHeight="11025"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="12915" windowHeight="11025" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ChoixMultiples" sheetId="1" r:id="rId1"/>
@@ -971,30 +971,30 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1299,7 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1315,13 +1315,13 @@
         <v>214</v>
       </c>
       <c r="B1" s="33"/>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1511,15 +1511,15 @@
         <v>212</v>
       </c>
       <c r="C1" s="19"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1776,12 +1776,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="42" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="36" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" customWidth="1"/>
     <col min="4" max="15" width="11.42578125" style="11"/>
   </cols>
@@ -1790,29 +1790,29 @@
       <c r="A1" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="40" t="s">
         <v>222</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="35" t="s">
         <v>237</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1862,7 +1862,7 @@
       <c r="A3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="35">
         <v>3</v>
       </c>
       <c r="C3" s="30" t="s">
@@ -1884,7 +1884,7 @@
       <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="1:17" ht="90" x14ac:dyDescent="0.25">
-      <c r="B4" s="42">
+      <c r="B4" s="36">
         <v>3</v>
       </c>
       <c r="C4" s="31" t="s">
@@ -1907,7 +1907,7 @@
       <c r="A5" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="37">
         <v>1</v>
       </c>
       <c r="C5" s="32" t="s">
@@ -1960,13 +1960,13 @@
       <c r="A1" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="41" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2201,13 +2201,13 @@
       <c r="E11" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2225,13 +2225,13 @@
       <c r="E12" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -2246,13 +2246,13 @@
       <c r="E13" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -2267,13 +2267,13 @@
       <c r="E14" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -2288,13 +2288,13 @@
       <c r="E15" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2422,15 +2422,15 @@
       <c r="C1" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">

</xml_diff>